<commit_message>
push merged code between Hari and Joseph
</commit_message>
<xml_diff>
--- a/Menu Items.xlsx
+++ b/Menu Items.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HariRaval/Desktop/expresso/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josephkim/Documents/GitHub/expresso/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB2350F-5A9C-E94E-A8E0-B094B4EA0089}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83758473-EE65-B94F-8A8E-C990AE2FA31D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19340" xr2:uid="{F392BF0F-2D18-0A4B-8C07-877493C8F80B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15960" xr2:uid="{F392BF0F-2D18-0A4B-8C07-877493C8F80B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="67">
   <si>
     <t>Latte</t>
   </si>
@@ -78,18 +78,12 @@
     <t>Scone</t>
   </si>
   <si>
-    <t>Bar</t>
-  </si>
-  <si>
     <t>Cookie</t>
   </si>
   <si>
     <t>Brownie</t>
   </si>
   <si>
-    <t>Caramel Crack</t>
-  </si>
-  <si>
     <t>Cinnamon Roll</t>
   </si>
   <si>
@@ -165,9 +159,6 @@
     <t>Did someone say minty mocha?</t>
   </si>
   <si>
-    <t>The perfect snack.</t>
-  </si>
-  <si>
     <t>I'm so cool.</t>
   </si>
   <si>
@@ -190,9 +181,6 @@
   </si>
   <si>
     <t>Brownie points.</t>
-  </si>
-  <si>
-    <t>Got sweets?</t>
   </si>
   <si>
     <t>On a roll.</t>
@@ -669,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7880B88-B6EE-7541-B2CA-748C503D23CF}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -683,7 +671,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>4</v>
@@ -692,10 +680,10 @@
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G1" s="1"/>
     </row>
@@ -704,19 +692,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2" s="3">
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G2" s="1"/>
     </row>
@@ -725,19 +713,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D3" s="5">
         <v>2.5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G3" s="1"/>
     </row>
@@ -747,7 +735,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>0</v>
@@ -756,20 +744,20 @@
         <v>3.5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
-        <f t="shared" ref="A5:A46" si="0">A4+1</f>
+        <f t="shared" ref="A5:A44" si="0">A4+1</f>
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>1</v>
@@ -778,10 +766,10 @@
         <v>2.5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G5" s="1"/>
     </row>
@@ -791,7 +779,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>2</v>
@@ -800,10 +788,10 @@
         <v>2.5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G6" s="1"/>
     </row>
@@ -813,7 +801,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>3</v>
@@ -822,10 +810,10 @@
         <v>3</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G7" s="1"/>
     </row>
@@ -835,19 +823,19 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D8" s="5">
         <v>2.5</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G8" s="1"/>
     </row>
@@ -857,19 +845,19 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D9" s="5">
         <v>3</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="G9" s="1"/>
     </row>
@@ -879,19 +867,19 @@
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D10" s="5">
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G10" s="1"/>
     </row>
@@ -901,19 +889,19 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D11" s="5">
         <v>2.5</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G11" s="1"/>
     </row>
@@ -923,19 +911,19 @@
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D12" s="5">
         <v>4</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -945,19 +933,19 @@
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D13" s="5">
         <v>4.5</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="G13" s="1"/>
     </row>
@@ -967,19 +955,19 @@
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D14" s="5">
         <v>3</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G14" s="1"/>
     </row>
@@ -989,19 +977,19 @@
         <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D15" s="5">
         <v>3.5</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G15" s="1"/>
     </row>
@@ -1011,19 +999,19 @@
         <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D16" s="3">
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G16" s="1"/>
     </row>
@@ -1033,19 +1021,19 @@
         <v>15</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D17" s="5">
         <v>2.5</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G17" s="1"/>
     </row>
@@ -1055,19 +1043,19 @@
         <v>16</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D18" s="5">
         <v>3.5</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G18" s="1"/>
     </row>
@@ -1077,19 +1065,19 @@
         <v>17</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D19" s="5">
         <v>4</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G19" s="1"/>
     </row>
@@ -1099,19 +1087,19 @@
         <v>18</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D20" s="5">
         <v>2.5</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G20" s="1"/>
     </row>
@@ -1121,19 +1109,19 @@
         <v>19</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D21" s="5">
         <v>3</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G21" s="1"/>
     </row>
@@ -1143,19 +1131,19 @@
         <v>20</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D22" s="5">
         <v>2</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G22" s="1"/>
     </row>
@@ -1165,19 +1153,19 @@
         <v>21</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D23" s="5">
         <v>2.5</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G23" s="1"/>
     </row>
@@ -1187,19 +1175,19 @@
         <v>22</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D24" s="5">
         <v>4</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G24" s="1"/>
     </row>
@@ -1209,19 +1197,19 @@
         <v>23</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D25" s="5">
         <v>4.5</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G25" s="1"/>
     </row>
@@ -1231,19 +1219,19 @@
         <v>24</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D26" s="3">
         <v>1.5</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G26" s="1"/>
     </row>
@@ -1253,19 +1241,19 @@
         <v>25</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D27" s="5">
         <v>2</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G27" s="1"/>
     </row>
@@ -1275,19 +1263,19 @@
         <v>26</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D28" s="5">
         <v>4</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G28" s="1"/>
     </row>
@@ -1297,19 +1285,19 @@
         <v>27</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D29" s="5">
         <v>4.5</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G29" s="1"/>
     </row>
@@ -1319,19 +1307,19 @@
         <v>28</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D30" s="5">
         <v>4</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G30" s="1"/>
     </row>
@@ -1341,19 +1329,19 @@
         <v>29</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D31" s="5">
         <v>4.5</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G31" s="1"/>
     </row>
@@ -1363,7 +1351,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>6</v>
@@ -1372,10 +1360,10 @@
         <v>0.5</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G32" s="1"/>
     </row>
@@ -1385,7 +1373,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C33" s="11" t="s">
         <v>7</v>
@@ -1394,10 +1382,10 @@
         <v>0.5</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G33" s="1"/>
     </row>
@@ -1407,7 +1395,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C34" s="11" t="s">
         <v>8</v>
@@ -1416,10 +1404,10 @@
         <v>0.5</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G34" s="1"/>
     </row>
@@ -1429,7 +1417,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C35" s="11" t="s">
         <v>9</v>
@@ -1438,10 +1426,10 @@
         <v>1</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G35" s="1"/>
     </row>
@@ -1451,7 +1439,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>10</v>
@@ -1460,10 +1448,10 @@
         <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G36" s="1"/>
     </row>
@@ -1473,7 +1461,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C37" s="11" t="s">
         <v>11</v>
@@ -1482,10 +1470,10 @@
         <v>1</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G37" s="1"/>
     </row>
@@ -1495,7 +1483,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C38" s="12" t="s">
         <v>12</v>
@@ -1504,10 +1492,10 @@
         <v>3</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G38" s="1"/>
     </row>
@@ -1517,19 +1505,19 @@
         <v>37</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D39" s="5">
         <v>3.25</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G39" s="1"/>
     </row>
@@ -1539,7 +1527,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>13</v>
@@ -1548,10 +1536,10 @@
         <v>3</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G40" s="1"/>
     </row>
@@ -1561,7 +1549,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>14</v>
@@ -1570,10 +1558,10 @@
         <v>3</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G41" s="1"/>
     </row>
@@ -1583,19 +1571,19 @@
         <v>40</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>15</v>
       </c>
       <c r="D42" s="5">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="G42" s="1"/>
     </row>
@@ -1604,20 +1592,20 @@
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="B43" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C43" s="9" t="s">
+      <c r="B43" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D43" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="G43" s="1"/>
     </row>
@@ -1626,65 +1614,27 @@
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="B44" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C44" s="11" t="s">
+      <c r="B44" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D44" s="5">
-        <v>3</v>
+      <c r="D44" s="14">
+        <v>3.25</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G44" s="1"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D45" s="5">
-        <v>3.5</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F45" s="8" t="s">
-        <v>53</v>
-      </c>
       <c r="G45" s="1"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="B46" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C46" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D46" s="14">
-        <v>3.25</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F46" s="8" t="s">
-        <v>54</v>
-      </c>
       <c r="G46" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update all headers and upload sendmail.py
</commit_message>
<xml_diff>
--- a/Menu Items.xlsx
+++ b/Menu Items.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josephkim/Documents/GitHub/expresso/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/HariRaval/Desktop/expresso/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83758473-EE65-B94F-8A8E-C990AE2FA31D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D83273-7D43-7A49-985B-163D06FDC5C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15960" xr2:uid="{F392BF0F-2D18-0A4B-8C07-877493C8F80B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{F392BF0F-2D18-0A4B-8C07-877493C8F80B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="94">
   <si>
     <t>Latte</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Macchiato</t>
   </si>
   <si>
-    <t>Capuccino</t>
-  </si>
-  <si>
     <t>item</t>
   </si>
   <si>
@@ -232,6 +229,90 @@
   </si>
   <si>
     <t>Chocolate Croissant</t>
+  </si>
+  <si>
+    <t>Cappuccino</t>
+  </si>
+  <si>
+    <t>definition</t>
+  </si>
+  <si>
+    <t>No definition</t>
+  </si>
+  <si>
+    <t>Hot drink made from the roasted and ground seeds (coffee beans) of a tropical shrub</t>
+  </si>
+  <si>
+    <t>Espresso mixed with hot or steamed milk</t>
+  </si>
+  <si>
+    <t>Strong black coffee made by forcing steam through ground coffee beans</t>
+  </si>
+  <si>
+    <t>Espresso with some foamy, steamed milk</t>
+  </si>
+  <si>
+    <t>Coffee made with milk that has been foamed up with pressurized steam</t>
+  </si>
+  <si>
+    <t>Drink made up of espresso diluted with hot water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hot drink made by infusing the dried crushed leaves of the tea plant in boiling water </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hot drink made from a blend of spices simmered in milk </t>
+  </si>
+  <si>
+    <t>Hot drink made with milk or water and chocolate or powdered chocolate</t>
+  </si>
+  <si>
+    <t>Chilled coffee, typically sweetened or flavored and served over ice</t>
+  </si>
+  <si>
+    <t>Eespresso and chilled milk poured over ice</t>
+  </si>
+  <si>
+    <t>Espresso and chilled milk poured over ice</t>
+  </si>
+  <si>
+    <t>Drink of espresso diluted with cold water</t>
+  </si>
+  <si>
+    <t>Chilled drink of sweetened tea, typically flavored with lemon</t>
+  </si>
+  <si>
+    <t>Tea mixed with milk and ice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drink made with creamy steamed milk, topped with flavored syrup </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coffee made with a mix of fall spice flavors and steamed milk  </t>
+  </si>
+  <si>
+    <t>Drink made with steamed milk, sweet mocha sauce and peppermint-flavored syrup</t>
+  </si>
+  <si>
+    <t>A flakey French bread / pastry made with butter</t>
+  </si>
+  <si>
+    <t>A chocolate flakey French bread / pastry made with butter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A small domed cake made from batter </t>
+  </si>
+  <si>
+    <t>A small biscuit-like cake</t>
+  </si>
+  <si>
+    <t>A small sweet baked good primarily made from flour and sugar</t>
+  </si>
+  <si>
+    <t>A small, sweet square of chocolate cake</t>
+  </si>
+  <si>
+    <t>A rolled pastry flavored with cinnamon and sugar</t>
   </si>
 </sst>
 </file>
@@ -657,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7880B88-B6EE-7541-B2CA-748C503D23CF}">
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -666,68 +747,74 @@
     <col min="2" max="2" width="36.33203125" customWidth="1"/>
     <col min="3" max="3" width="24.83203125" customWidth="1"/>
     <col min="6" max="6" width="35.6640625" customWidth="1"/>
-    <col min="7" max="7" width="54" customWidth="1"/>
+    <col min="7" max="7" width="76.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="3">
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G2" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" s="5">
         <v>2.5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G3" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -735,7 +822,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>0</v>
@@ -744,12 +831,14 @@
         <v>3.5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="1"/>
+        <v>37</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -757,7 +846,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>1</v>
@@ -766,12 +855,14 @@
         <v>2.5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="1"/>
+        <v>35</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -779,7 +870,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>2</v>
@@ -788,12 +879,14 @@
         <v>2.5</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G6" s="1"/>
+        <v>55</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -801,21 +894,23 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="D7" s="5">
         <v>3</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7" s="1"/>
+        <v>42</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -823,21 +918,23 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="5">
         <v>2.5</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G8" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -845,21 +942,23 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D9" s="5">
         <v>3</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -867,21 +966,23 @@
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="5">
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G10" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -889,21 +990,23 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="5">
         <v>2.5</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G11" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -911,21 +1014,23 @@
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="5">
         <v>4</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -933,21 +1038,23 @@
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D13" s="5">
         <v>4.5</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G13" s="1"/>
+        <v>58</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -955,21 +1062,23 @@
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D14" s="5">
         <v>3</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -977,21 +1086,23 @@
         <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D15" s="5">
         <v>3.5</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" s="1"/>
+        <v>39</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -999,21 +1110,23 @@
         <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" s="3">
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G16" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
@@ -1021,21 +1134,23 @@
         <v>15</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D17" s="5">
         <v>2.5</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G17" s="1"/>
+        <v>41</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
@@ -1043,21 +1158,23 @@
         <v>16</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D18" s="5">
         <v>3.5</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G18" s="1"/>
+        <v>43</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
@@ -1065,21 +1182,23 @@
         <v>17</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" s="5">
         <v>4</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G19" s="1"/>
+        <v>43</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
@@ -1087,21 +1206,23 @@
         <v>18</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20" s="5">
         <v>2.5</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G20" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
@@ -1109,21 +1230,23 @@
         <v>19</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D21" s="5">
         <v>3</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G21" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
@@ -1131,21 +1254,23 @@
         <v>20</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D22" s="5">
         <v>2</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G22" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
@@ -1153,21 +1278,23 @@
         <v>21</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D23" s="5">
         <v>2.5</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G23" s="1"/>
+        <v>38</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
@@ -1175,21 +1302,23 @@
         <v>22</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D24" s="5">
         <v>4</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="G24" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
@@ -1197,21 +1326,23 @@
         <v>23</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D25" s="5">
         <v>4.5</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="G25" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
@@ -1219,21 +1350,23 @@
         <v>24</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D26" s="3">
         <v>1.5</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G26" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
@@ -1241,21 +1374,23 @@
         <v>25</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D27" s="5">
         <v>2</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G27" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
@@ -1263,21 +1398,23 @@
         <v>26</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D28" s="5">
         <v>4</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G28" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
@@ -1285,21 +1422,23 @@
         <v>27</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D29" s="5">
         <v>4.5</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G29" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
@@ -1307,21 +1446,23 @@
         <v>28</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D30" s="5">
         <v>4</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G30" s="1"/>
+        <v>40</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
@@ -1329,21 +1470,23 @@
         <v>29</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D31" s="5">
         <v>4.5</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G31" s="1"/>
+        <v>40</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
@@ -1351,21 +1494,23 @@
         <v>30</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D32" s="3">
         <v>0.5</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G32" s="1"/>
+        <v>52</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
@@ -1373,21 +1518,23 @@
         <v>31</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D33" s="5">
         <v>0.5</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G33" s="1"/>
+        <v>52</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
@@ -1395,21 +1542,23 @@
         <v>32</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D34" s="5">
         <v>0.5</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G34" s="1"/>
+        <v>52</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
@@ -1417,21 +1566,23 @@
         <v>33</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D35" s="5">
         <v>1</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G35" s="1"/>
+        <v>52</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
@@ -1439,21 +1590,23 @@
         <v>34</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D36" s="5">
         <v>1</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G36" s="1"/>
+        <v>52</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
@@ -1461,21 +1614,23 @@
         <v>35</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D37" s="5">
         <v>1</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G37" s="1"/>
+        <v>52</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
@@ -1483,21 +1638,23 @@
         <v>36</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D38" s="3">
         <v>3</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F38" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G38" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
@@ -1505,21 +1662,23 @@
         <v>37</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D39" s="5">
         <v>3.25</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F39" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="G39" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="G39" s="8" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
@@ -1527,21 +1686,23 @@
         <v>38</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D40" s="5">
         <v>3</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F40" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="G40" s="1"/>
+        <v>46</v>
+      </c>
+      <c r="G40" s="8" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
@@ -1549,21 +1710,23 @@
         <v>39</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D41" s="5">
         <v>3</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="G41" s="1"/>
+        <v>47</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
@@ -1571,21 +1734,23 @@
         <v>40</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D42" s="5">
         <v>2</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="G42" s="1"/>
+        <v>62</v>
+      </c>
+      <c r="G42" s="8" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
@@ -1593,21 +1758,23 @@
         <v>41</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D43" s="5">
         <v>3</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="G43" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
@@ -1615,21 +1782,23 @@
         <v>42</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D44" s="14">
         <v>3.25</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="G44" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="G44" s="8" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G45" s="1"/>

</xml_diff>